<commit_message>
Bunt updates finish 2017 series 1
</commit_message>
<xml_diff>
--- a/buntseries2.xlsx
+++ b/buntseries2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13816" uniqueCount="9393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13800" uniqueCount="9387">
   <si>
     <t xml:space="preserve"> Joey Gallo</t>
   </si>
@@ -28161,52 +28161,34 @@
     <t>0B-SU-eAGCKuiVW9IaF9vTmExYnM</t>
   </si>
   <si>
-    <t>Jedd Gyorko.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuiQ3dWeXczZTJfSWs</t>
   </si>
   <si>
-    <t>Austin Hedges.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuiYlgzV2JFSkVZd0k</t>
   </si>
   <si>
-    <t>Ubaldo Jimenez.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuiRUR1S3prdnlFRkE</t>
   </si>
   <si>
     <t>0B-SU-eAGCKuiNVpqZmgtRHQtRW8</t>
   </si>
   <si>
-    <t>Colin McHugh.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuidXNKX1Z6NXVIR3M</t>
   </si>
   <si>
-    <t>Stephen Piscotty.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuidHdUdGpNODJsdUE</t>
   </si>
   <si>
-    <t>Trea Turner.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuiZGs3cTVtS1R3bUE</t>
   </si>
   <si>
-    <t>Branden Maurer.png</t>
-  </si>
-  <si>
     <t>0B-SU-eAGCKuiejM5S194SFVTa1U</t>
   </si>
   <si>
-    <t>Dbacks</t>
+    <t>0B-SU-eAGCKuiOFBIRk1tWDRvbW8</t>
+  </si>
+  <si>
+    <t>0B-SU-eAGCKuiRElLM2RUZjJLRU0</t>
   </si>
 </sst>
 </file>
@@ -29061,8 +29043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F395"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B248" sqref="B248"/>
+    <sheetView tabSelected="1" topLeftCell="A387" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B395" sqref="B395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29333,7 +29315,7 @@
         <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>9385</v>
+        <v>9381</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -29702,13 +29684,16 @@
         <v>543</v>
       </c>
       <c r="B98" t="s">
-        <v>9378</v>
+        <v>9377</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>187</v>
       </c>
+      <c r="B99" t="s">
+        <v>9385</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -29739,7 +29724,7 @@
         <v>547</v>
       </c>
       <c r="B103" t="s">
-        <v>9387</v>
+        <v>9382</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -29978,7 +29963,7 @@
         <v>9052</v>
       </c>
       <c r="B142" t="s">
-        <v>9383</v>
+        <v>9380</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -30507,7 +30492,7 @@
         <v>581</v>
       </c>
       <c r="B224" t="s">
-        <v>9389</v>
+        <v>9383</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -30568,7 +30553,7 @@
         <v>328</v>
       </c>
       <c r="B235" t="s">
-        <v>9382</v>
+        <v>9379</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -30629,7 +30614,7 @@
         <v>4195</v>
       </c>
       <c r="B246" t="s">
-        <v>9380</v>
+        <v>9378</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -30645,7 +30630,7 @@
         <v>9080</v>
       </c>
       <c r="B248" t="s">
-        <v>9391</v>
+        <v>9384</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -31618,6 +31603,9 @@
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>257</v>
+      </c>
+      <c r="B395" t="s">
+        <v>9386</v>
       </c>
     </row>
   </sheetData>
@@ -37310,10 +37298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37321,80 +37309,7 @@
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9384</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5381</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9377</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9386</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5402</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8374</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5403</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9388</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9381</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5377</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9379</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9390</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5384</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sortState ref="A2:C10">
     <sortCondition ref="C2:C10"/>
   </sortState>

</xml_diff>